<commit_message>
update export htmltotext exercises
</commit_message>
<xml_diff>
--- a/src/public/exports/thong-ke-danh-sach-cau-hoi-bai-cuc-tri-cua-ham-so.xlsx
+++ b/src/public/exports/thong-ke-danh-sach-cau-hoi-bai-cuc-tri-cua-ham-so.xlsx
@@ -417,7 +417,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>&lt;p&gt;1+1=&lt;/p&gt;</v>
+        <v>1+1=</v>
       </c>
       <c r="C2" t="str">
         <v>1</v>
@@ -438,7 +438,7 @@
         <v>abc</v>
       </c>
       <c r="I2" t="str">
-        <v>&lt;p&gt;abc&lt;/p&gt;</v>
+        <v>abc</v>
       </c>
       <c r="J2" t="str">
         <v>nhận biết</v>
@@ -476,12 +476,14 @@
         <v>thông hiểu</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" xml:space="preserve">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <v>&lt;p&gt;&lt;math xmlns="http://www.w3.org/1998/Math/MathML"&gt;&lt;mfrac&gt;&lt;mn&gt;1&lt;/mn&gt;&lt;mn&gt;2&lt;/mn&gt;&lt;/mfrac&gt;&lt;mo&gt;&amp;nbsp;&lt;/mo&gt;&lt;mo&gt;+&lt;/mo&gt;&lt;mo&gt;&amp;nbsp;&lt;/mo&gt;&lt;mn&gt;1&lt;/mn&gt;&lt;mo&gt;&amp;nbsp;&lt;/mo&gt;&lt;mo&gt;=&lt;/mo&gt;&lt;mo&gt;&amp;nbsp;&lt;/mo&gt;&lt;/math&gt;&lt;/p&gt;</v>
+      <c r="B4" t="str" xml:space="preserve">
+        <v xml:space="preserve">12 + 1 = 
+2 3  4  333 
+x3 + 2x2 - 1</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
@@ -502,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="str">
-        <v>&lt;p&gt;1&lt;/p&gt;</v>
+        <v>1</v>
       </c>
       <c r="J4" t="str">
         <v>nhận biết</v>

</xml_diff>